<commit_message>
Einfügen der Tabellen durch Sebastian Golchert
Anlegen eines Issues für Fragen zu den Datentypen
</commit_message>
<xml_diff>
--- a/Relationales Modell.xlsx
+++ b/Relationales Modell.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\Studium\Softwareprojekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgolc\Documents\TEAMUNIQUE\Projekt-Bibo-MarkusW95-patch-3\Projekt-Bibo-MarkusW95-patch-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B640707-4B71-4B64-B0B1-649B42180124}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE34AFCD-A0FE-4F39-AE7E-22D4B858C0EF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{E4186542-6DEA-4CBB-AC98-2E97943477EF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="12953" activeTab="1" xr2:uid="{E4186542-6DEA-4CBB-AC98-2E97943477EF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Markus" sheetId="1" r:id="rId1"/>
+    <sheet name="Sebastian" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>int</t>
   </si>
@@ -96,6 +97,36 @@
   </si>
   <si>
     <t>beginnend bei 1000</t>
+  </si>
+  <si>
+    <t>Bauteile</t>
+  </si>
+  <si>
+    <t>Roboterkomponenten</t>
+  </si>
+  <si>
+    <t>Roboter</t>
+  </si>
+  <si>
+    <t>RoboterID</t>
+  </si>
+  <si>
+    <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>Materialkosten</t>
+  </si>
+  <si>
+    <t>Produktionskosten</t>
+  </si>
+  <si>
+    <t>TeileNr</t>
+  </si>
+  <si>
+    <t>varchar[?]</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -479,21 +510,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F81AA6-5C7C-440A-A2D4-5698364E7091}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="83.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="83.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -510,13 +541,13 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -533,7 +564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -544,12 +575,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -563,7 +594,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -574,12 +605,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
@@ -599,7 +630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -610,7 +641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="3"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -618,7 +649,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="4"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -626,7 +657,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -634,7 +665,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -642,7 +673,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -650,7 +681,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -658,7 +689,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -666,7 +697,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -674,7 +705,7 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -682,7 +713,7 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -690,7 +721,7 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -698,7 +729,7 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -710,4 +741,220 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9768B04-7F66-44AE-B6F1-CB75DB93B2F4}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>